<commit_message>
AMP and BFI, IAT Task completed
</commit_message>
<xml_diff>
--- a/implicit evaluations study/data/processed/data_processed_codebook.xlsx
+++ b/implicit evaluations study/data/processed/data_processed_codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tinap\GitHub\dpm-assignments\week 10-11 update\implicit evaluations study\data\processed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tina\Documents\GitHub\dpm-assignments\implicit evaluations study\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBEA16B-BABF-47BE-8328-BB4A4B0DFEED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48A2622-23AD-4411-817F-5B80F6EF35CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10710" yWindow="0" windowWidth="10980" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -73,21 +73,6 @@
     <t>exclude_participant</t>
   </si>
   <si>
-    <t>a code so that the various data can be assigned to the respective participants - every participant has an own code</t>
-  </si>
-  <si>
-    <t>the date on which the data was collected from the respective participant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">the exact time when the participants took part in the experiment  </t>
-  </si>
-  <si>
-    <t>the age of the respective participant (given in years!)</t>
-  </si>
-  <si>
-    <t>the gender that the respective participant identifies as</t>
-  </si>
-  <si>
     <t xml:space="preserve">Scale 1-7 the evaluation of the stimuli in relation to liking. </t>
   </si>
   <si>
@@ -116,6 +101,21 @@
   </si>
   <si>
     <t>Participants were excluded if they had more than 0.10 in the "proportion_fast_trials". - too problematic, therefore excluded (excluded vs. included)</t>
+  </si>
+  <si>
+    <t>A code so that the various data can be assigned to the respective participants - every participant has an own code.</t>
+  </si>
+  <si>
+    <t>The date on which the data was collected from the respective participant.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The exact time when the participants took part in the experiment. </t>
+  </si>
+  <si>
+    <t>The age of the respective participant (given in years!).</t>
+  </si>
+  <si>
+    <t>The gender that the respective participant identifies as.</t>
   </si>
 </sst>
 </file>
@@ -461,12 +461,12 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,124 +474,124 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>